<commit_message>
last update tyol 21012020
</commit_message>
<xml_diff>
--- a/Genbot.UI/Assets/Upload/turan/morhipo de.xlsx
+++ b/Genbot.UI/Assets/Upload/turan/morhipo de.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbalt\Desktop\Günerler Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbalt\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C6EFE8-6C44-446D-A839-1656EE8839F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1C150D-BC84-4E99-8008-B2AFC6859CD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -26,13 +26,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF333333"/>
+      <name val="Source_sans_proregular"/>
     </font>
   </fonts>
   <fills count="2">
@@ -57,7 +62,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -338,93 +343,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:A16"/>
+  <dimension ref="A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="18.75">
       <c r="A2" s="1">
-        <v>3367729019001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>3367729018943</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3605540856703</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3605540856635</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>3367729018981</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>3605540946183</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>3367729018974</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>3367729021066</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>3614271099853</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>737052933269</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>737052933221</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>3614229371611</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>3614228830515</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>3614228830393</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>3367729021035</v>
+        <v>3348901250146</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>